<commit_message>
User stories updated for Sprint 2
</commit_message>
<xml_diff>
--- a/Product_Backlog/User Stories.xlsx
+++ b/Product_Backlog/User Stories.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaylawallace/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Documents/Agile_Development_Project1/Product_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786E4219-04C7-CB4C-A110-A8CE48F47042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6407BE-38D6-3940-8F6A-102A9A70C330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile User Stories" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Priority" localSheetId="0">'Agile User Stories'!$J$4:$J$25</definedName>
-    <definedName name="Status" localSheetId="0">'Agile User Stories'!$K$4:$K$25</definedName>
+    <definedName name="Priority" localSheetId="0">'Agile User Stories'!$J$4:$J$23</definedName>
+    <definedName name="Status" localSheetId="0">'Agile User Stories'!$K$4:$K$23</definedName>
     <definedName name="YesNo" localSheetId="0">#REF!</definedName>
-    <definedName name="Z_B0192A1B_C231_4E6E_8016_635727756B48_.wvu.FilterData" localSheetId="0" hidden="1">'Agile User Stories'!$A$2:$P$25</definedName>
+    <definedName name="Z_B0192A1B_C231_4E6E_8016_635727756B48_.wvu.FilterData" localSheetId="0" hidden="1">'Agile User Stories'!$A$2:$P$23</definedName>
     <definedName name="Z_C48613A2_CEF0_4133_8558_F313CB0F2FEB_.wvu.FilterData" localSheetId="0" hidden="1">'Agile User Stories'!$B$2:$H$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{B0192A1B-C231-4E6E-8016-635727756B48}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{B0192A1B-C231-4E6E-8016-635727756B48}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>USER STORIES</t>
   </si>
@@ -67,73 +67,10 @@
     <t>CONFIRMATION</t>
   </si>
   <si>
-    <t>A user can search based on code.</t>
-  </si>
-  <si>
-    <t>A user can search based on procedure.</t>
-  </si>
-  <si>
-    <t>A user can search based on condition.</t>
-  </si>
-  <si>
-    <t>A user can search based on live location.</t>
-  </si>
-  <si>
-    <t>A user can search based on location input.</t>
-  </si>
-  <si>
-    <t>A user can search based on a description of a condition.</t>
-  </si>
-  <si>
-    <t>A user can search based on a description of a procedure.</t>
-  </si>
-  <si>
-    <t>A user can order the search results based on price.</t>
-  </si>
-  <si>
-    <t>A user can order the search results based on distance.</t>
-  </si>
-  <si>
-    <t>A user can view the output of a search as a list.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A user can view the search results on a map. </t>
-  </si>
-  <si>
-    <t>A user can see the price information on a placeholder for each result on the map.</t>
-  </si>
-  <si>
     <t>As a programmer, I want to find an API to support Google Maps for live location services.</t>
   </si>
   <si>
     <t>As a programmer, I want the data to be stored in a database so that all the data is easy to access for any user.</t>
-  </si>
-  <si>
-    <t>A user can set a price range for their search.</t>
-  </si>
-  <si>
-    <t>A user can set a distance range for their search.</t>
-  </si>
-  <si>
-    <t>A user can order the search results based on a ranking which is a combination of price, distance and user feedback.</t>
-  </si>
-  <si>
-    <t>The purchaser can delete data from the existing data set.</t>
-  </si>
-  <si>
-    <t>The purchaser can load new data from the existing data set.</t>
-  </si>
-  <si>
-    <t>The purchaser can update existing data.</t>
-  </si>
-  <si>
-    <t>The purchaser can add data to the existing data set.</t>
-  </si>
-  <si>
-    <t>A user can navigate with a keyboard.</t>
-  </si>
-  <si>
-    <t>A user can view the data regardless of colour blindness.</t>
   </si>
   <si>
     <t>As a programmer, I would like to create a webpage as the main interface to allow the user easy and effective access to all the data.</t>
@@ -288,12 +225,78 @@
   <si>
     <t xml:space="preserve">Test when clicking on a marker than the placeholder shows the price information from the data set provided. </t>
   </si>
+  <si>
+    <t>As a user, I can search based on code.</t>
+  </si>
+  <si>
+    <t>As a user, I can search based on procedure.</t>
+  </si>
+  <si>
+    <t>As a user, I can search based on live location.</t>
+  </si>
+  <si>
+    <t>As a user, I can search based on location input.</t>
+  </si>
+  <si>
+    <t>As a user, I can search based on a description of a procedure.</t>
+  </si>
+  <si>
+    <t>As a user, I can order the search results based on price.</t>
+  </si>
+  <si>
+    <t>As a user, I can order the search results based on distance.</t>
+  </si>
+  <si>
+    <t>As a user, I can view the output of a search as a list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I can view the search results on a map. </t>
+  </si>
+  <si>
+    <t>As a user, I can see the price information on a placeholder for each result on the map.</t>
+  </si>
+  <si>
+    <t>As a user, I can set a price range for their search.</t>
+  </si>
+  <si>
+    <t>As a user, I can set a distance range for their search.</t>
+  </si>
+  <si>
+    <t>As a user, I can order the search results based on a ranking which is a combination of price, distance and user feedback.</t>
+  </si>
+  <si>
+    <t>As a purchaser, I can delete data from the existing data set.</t>
+  </si>
+  <si>
+    <t>As a purchaser, I can load new data from the existing data set.</t>
+  </si>
+  <si>
+    <t>As a purchaser, I can update existing data.</t>
+  </si>
+  <si>
+    <t>As a purchaser, I can add data to the existing data set.</t>
+  </si>
+  <si>
+    <t>As a user, I can navigate with a keyboard.</t>
+  </si>
+  <si>
+    <t>As a user, I can view the data regardless of colour blindness.</t>
+  </si>
+  <si>
+    <t>As a programmer, I would like to optimise a webpage based on user feedback</t>
+  </si>
+  <si>
+    <t>As a programmer, I want to create unit tests for all existing functionality so that I can ensure further development doesn't break any existing code</t>
+  </si>
+  <si>
+    <t>As a programmer, I want to store longtitude/latitude coordinates for each hospital address in the database a this allows for quicker fetches</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -351,12 +354,6 @@
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -525,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -557,9 +554,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -570,12 +564,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -591,38 +579,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,8 +839,8 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="81" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -917,32 +911,32 @@
     </row>
     <row r="3" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="11">
+      <c r="B3" s="33">
         <f t="shared" ref="B3:B28" si="0">ROW()-2</f>
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="28">
+      <c r="C3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="25">
         <v>9</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="26">
         <v>1</v>
       </c>
-      <c r="F3" s="29">
-        <f t="shared" ref="F3:F27" si="1">ROUND((D3/E3),0)</f>
+      <c r="F3" s="26">
+        <f t="shared" ref="F3:F28" si="1">ROUND((D3/E3),0)</f>
         <v>9</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>33</v>
+      <c r="G3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>12</v>
       </c>
       <c r="I3" s="9"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
       <c r="L3" s="1"/>
       <c r="M3" s="10"/>
       <c r="N3" s="5"/>
@@ -951,32 +945,32 @@
     </row>
     <row r="4" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="11">
+      <c r="B4" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="29">
+      <c r="C4" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="26">
         <v>10</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="26">
         <v>1</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="26">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>35</v>
+      <c r="G4" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>14</v>
       </c>
       <c r="I4" s="9"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="1"/>
       <c r="M4" s="10"/>
       <c r="N4" s="5"/>
@@ -985,32 +979,32 @@
     </row>
     <row r="5" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="11">
+      <c r="B5" s="33">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="29">
-        <v>10</v>
-      </c>
-      <c r="E5" s="29">
+      <c r="C5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="26">
+        <v>7</v>
+      </c>
+      <c r="E5" s="26">
+        <v>5</v>
+      </c>
+      <c r="F5" s="26">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F5" s="29">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>35</v>
+      <c r="G5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14"/>
       <c r="L5" s="1"/>
       <c r="M5" s="10"/>
       <c r="N5" s="5"/>
@@ -1019,32 +1013,32 @@
     </row>
     <row r="6" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="11">
+      <c r="B6" s="33">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="29">
-        <v>7</v>
-      </c>
-      <c r="E6" s="29">
+      <c r="C6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="26">
+        <v>9</v>
+      </c>
+      <c r="E6" s="26">
         <v>4</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>60</v>
+      <c r="G6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="1"/>
       <c r="M6" s="10"/>
       <c r="N6" s="5"/>
@@ -1053,32 +1047,32 @@
     </row>
     <row r="7" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-      <c r="B7" s="11">
+      <c r="B7" s="33">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="29">
-        <v>9</v>
-      </c>
-      <c r="E7" s="29">
-        <v>4</v>
-      </c>
-      <c r="F7" s="29">
+      <c r="C7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="26">
+        <v>6</v>
+      </c>
+      <c r="E7" s="26">
+        <v>2</v>
+      </c>
+      <c r="F7" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>59</v>
+        <v>3</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="15"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="14"/>
       <c r="L7" s="1"/>
       <c r="M7" s="10"/>
       <c r="N7" s="5"/>
@@ -1087,32 +1081,32 @@
     </row>
     <row r="8" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
-      <c r="B8" s="11">
+      <c r="B8" s="33">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="29">
-        <v>6</v>
-      </c>
-      <c r="E8" s="29">
-        <v>2</v>
-      </c>
-      <c r="F8" s="29">
+      <c r="C8" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="26">
+        <v>8</v>
+      </c>
+      <c r="E8" s="26">
+        <v>1</v>
+      </c>
+      <c r="F8" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>61</v>
+        <v>8</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="15"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="1"/>
       <c r="M8" s="10"/>
       <c r="N8" s="5"/>
@@ -1121,32 +1115,32 @@
     </row>
     <row r="9" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
-      <c r="B9" s="11">
+      <c r="B9" s="33">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="29">
-        <v>6</v>
-      </c>
-      <c r="E9" s="29">
-        <v>2</v>
-      </c>
-      <c r="F9" s="29">
+      <c r="C9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="26">
+        <v>8</v>
+      </c>
+      <c r="E9" s="26">
+        <v>1</v>
+      </c>
+      <c r="F9" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>61</v>
+        <v>8</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="I9" s="9"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="1"/>
       <c r="M9" s="10"/>
       <c r="N9" s="5"/>
@@ -1155,32 +1149,32 @@
     </row>
     <row r="10" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
-      <c r="B10" s="11">
+      <c r="B10" s="33">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="29">
-        <v>8</v>
-      </c>
-      <c r="E10" s="29">
-        <v>1</v>
-      </c>
-      <c r="F10" s="29">
+      <c r="C10" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="26">
+        <v>10</v>
+      </c>
+      <c r="E10" s="26">
+        <v>3</v>
+      </c>
+      <c r="F10" s="26">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>62</v>
+        <v>3</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="I10" s="9"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="14"/>
       <c r="L10" s="1"/>
       <c r="M10" s="10"/>
       <c r="N10" s="5"/>
@@ -1189,32 +1183,32 @@
     </row>
     <row r="11" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
-      <c r="B11" s="11">
+      <c r="B11" s="33">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="29">
+      <c r="C11" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="26">
+        <v>5</v>
+      </c>
+      <c r="E11" s="26">
         <v>8</v>
       </c>
-      <c r="E11" s="29">
+      <c r="F11" s="26">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F11" s="29">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>62</v>
+      <c r="G11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="14"/>
       <c r="L11" s="1"/>
       <c r="M11" s="10"/>
       <c r="N11" s="5"/>
@@ -1223,32 +1217,32 @@
     </row>
     <row r="12" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="11">
+      <c r="B12" s="33">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="29">
-        <v>10</v>
-      </c>
-      <c r="E12" s="29">
-        <v>3</v>
-      </c>
-      <c r="F12" s="29">
+      <c r="C12" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="26">
+        <v>4</v>
+      </c>
+      <c r="E12" s="26">
+        <v>5</v>
+      </c>
+      <c r="F12" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>53</v>
+        <v>1</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
+      <c r="K12" s="14"/>
       <c r="L12" s="1"/>
       <c r="M12" s="10"/>
       <c r="N12" s="5"/>
@@ -1257,32 +1251,32 @@
     </row>
     <row r="13" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
-      <c r="B13" s="11">
+      <c r="B13" s="33">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="29">
+      <c r="C13" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="26">
+        <v>7</v>
+      </c>
+      <c r="E13" s="26">
         <v>5</v>
       </c>
-      <c r="E13" s="29">
-        <v>7</v>
-      </c>
-      <c r="F13" s="29">
+      <c r="F13" s="26">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>65</v>
+      <c r="G13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="15"/>
+      <c r="K13" s="14"/>
       <c r="L13" s="1"/>
       <c r="M13" s="10"/>
       <c r="N13" s="5"/>
@@ -1291,168 +1285,163 @@
     </row>
     <row r="14" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
-      <c r="B14" s="11">
+      <c r="B14" s="33">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="29">
-        <v>4</v>
-      </c>
-      <c r="E14" s="29">
+      <c r="C14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="26">
+        <v>10</v>
+      </c>
+      <c r="E14" s="26">
         <v>6</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>68</v>
+        <v>2</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I14" s="9"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
       <c r="L14" s="1"/>
       <c r="M14" s="10"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" ht="108" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
-      <c r="B15" s="11">
+      <c r="B15" s="33">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="29">
-        <v>7</v>
-      </c>
-      <c r="E15" s="29">
-        <v>5</v>
-      </c>
-      <c r="F15" s="29">
+      <c r="C15" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="26">
+        <v>2</v>
+      </c>
+      <c r="E15" s="26">
+        <v>2</v>
+      </c>
+      <c r="F15" s="26">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>44</v>
+      <c r="G15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="I15" s="9"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
       <c r="L15" s="1"/>
       <c r="M15" s="10"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-      <c r="B16" s="11">
+      <c r="B16" s="33">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="29">
-        <v>10</v>
-      </c>
-      <c r="E16" s="29">
-        <v>6</v>
-      </c>
-      <c r="F16" s="29">
+      <c r="C16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="26">
+        <v>3</v>
+      </c>
+      <c r="E16" s="26">
+        <v>3</v>
+      </c>
+      <c r="F16" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="I16" s="9"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
       <c r="L16" s="1"/>
       <c r="M16" s="10"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" ht="108" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
-      <c r="B17" s="11">
+      <c r="B17" s="33">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="29">
-        <v>2</v>
-      </c>
-      <c r="E17" s="29">
-        <v>2</v>
-      </c>
-      <c r="F17" s="29">
+      <c r="C17" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="26">
+        <v>4</v>
+      </c>
+      <c r="E17" s="26">
+        <v>5</v>
+      </c>
+      <c r="F17" s="26">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>46</v>
+      <c r="G17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="1"/>
       <c r="M17" s="10"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
-      <c r="B18" s="11">
+      <c r="B18" s="33">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="26">
+        <v>1</v>
+      </c>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="29">
-        <v>3</v>
-      </c>
-      <c r="E18" s="29">
-        <v>3</v>
-      </c>
-      <c r="F18" s="29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="I18" s="9"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
       <c r="L18" s="1"/>
       <c r="M18" s="10"/>
       <c r="N18" s="5"/>
@@ -1461,32 +1450,27 @@
     </row>
     <row r="19" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
-      <c r="B19" s="11">
+      <c r="B19" s="33">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="29">
-        <v>4</v>
-      </c>
-      <c r="E19" s="29">
-        <v>5</v>
-      </c>
-      <c r="F19" s="29">
-        <f t="shared" si="1"/>
+      <c r="C19" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="26">
         <v>1</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>63</v>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="I19" s="9"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
       <c r="L19" s="1"/>
       <c r="M19" s="10"/>
       <c r="N19" s="5"/>
@@ -1495,27 +1479,27 @@
     </row>
     <row r="20" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
-      <c r="B20" s="11">
+      <c r="B20" s="33">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="29">
+      <c r="C20" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="26">
         <v>1</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>44</v>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="I20" s="9"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
       <c r="L20" s="1"/>
       <c r="M20" s="10"/>
       <c r="N20" s="5"/>
@@ -1524,27 +1508,27 @@
     </row>
     <row r="21" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="11">
+      <c r="B21" s="33">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C21" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="29">
+      <c r="C21" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="26">
         <v>1</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>44</v>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="I21" s="9"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="1"/>
       <c r="M21" s="10"/>
       <c r="N21" s="5"/>
@@ -1553,27 +1537,32 @@
     </row>
     <row r="22" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
-      <c r="B22" s="11">
+      <c r="B22" s="33">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="29">
+      <c r="C22" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="26">
+        <v>3</v>
+      </c>
+      <c r="E22" s="26">
         <v>1</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>44</v>
+      <c r="F22" s="26">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="I22" s="9"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
       <c r="L22" s="1"/>
       <c r="M22" s="10"/>
       <c r="N22" s="5"/>
@@ -1582,27 +1571,32 @@
     </row>
     <row r="23" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
-      <c r="B23" s="11">
+      <c r="B23" s="33">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="29">
-        <v>1</v>
-      </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>44</v>
+        <v>66</v>
+      </c>
+      <c r="D23" s="26">
+        <v>3</v>
+      </c>
+      <c r="E23" s="26">
+        <v>2</v>
+      </c>
+      <c r="F23" s="26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="I23" s="9"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
       <c r="L23" s="1"/>
       <c r="M23" s="10"/>
       <c r="N23" s="5"/>
@@ -1611,152 +1605,153 @@
     </row>
     <row r="24" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
-      <c r="B24" s="11">
+      <c r="B24" s="33">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C24" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="29">
-        <v>3</v>
-      </c>
-      <c r="E24" s="29">
-        <v>1</v>
-      </c>
-      <c r="F24" s="29">
+      <c r="C24" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="26">
+        <v>10</v>
+      </c>
+      <c r="E24" s="26">
+        <v>5</v>
+      </c>
+      <c r="F24" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="I24" s="9"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="10"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" ht="93" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
-      <c r="B25" s="11">
+      <c r="B25" s="33">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="29">
-        <v>3</v>
-      </c>
-      <c r="E25" s="29">
-        <v>2</v>
-      </c>
-      <c r="F25" s="29">
+      <c r="C25" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="27">
+        <v>10</v>
+      </c>
+      <c r="E25" s="27">
+        <v>7</v>
+      </c>
+      <c r="F25" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I25" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="5"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="10"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
-      <c r="B26" s="11">
+      <c r="B26" s="33">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="29">
+      <c r="C26" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="27">
+        <v>4</v>
+      </c>
+      <c r="E26" s="27">
+        <v>3</v>
+      </c>
+      <c r="F26" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+    </row>
+    <row r="27" spans="1:16" ht="86" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="1"/>
+      <c r="B27" s="33">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="27">
         <v>10</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E27" s="27">
         <v>5</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F27" s="26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G26" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="1:16" ht="112" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
-      <c r="B27" s="11">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="30">
-        <v>10</v>
-      </c>
-      <c r="E27" s="30">
-        <v>7</v>
-      </c>
-      <c r="F27" s="29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G27" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
     </row>
     <row r="28" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
-      <c r="B28" s="11">
+      <c r="B28" s="33">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="C28" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="27">
+        <v>8</v>
+      </c>
+      <c r="E28" s="27">
+        <v>5</v>
+      </c>
+      <c r="F28" s="26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -1785,32 +1780,32 @@
       <c r="P29" s="5"/>
     </row>
     <row r="30" spans="1:16" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
     </row>
     <row r="31" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -1823,12 +1818,12 @@
     <row r="32" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -2164,20 +2159,20 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="B2:H28" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H28">
-          <sortCondition descending="1" ref="D2:D28"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
     <customSheetView guid="{B0192A1B-C231-4E6E-8016-635727756B48}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A2:P25" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P25">
           <sortCondition descending="1" ref="D2:D25"/>
           <sortCondition ref="E2:E25"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="B2:H28" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H28">
+          <sortCondition descending="1" ref="D2:D28"/>
         </sortState>
       </autoFilter>
     </customSheetView>

</xml_diff>